<commit_message>
Update test de seis sombrero.xlsx
</commit_message>
<xml_diff>
--- a/test de seis sombrero.xlsx
+++ b/test de seis sombrero.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edferoca\Documents\GitHub\embebidos2019-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E81DBAB-D6AC-4494-A342-FD089193E6BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791E114E-6290-4E69-ACA4-D440BFCF4B5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="17">
   <si>
     <t>sombrero1</t>
   </si>
@@ -460,7 +460,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,9 +536,15 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>